<commit_message>
Updated the respiratory model to show improved alveoli recruitment with increased PEEP and added a new scenario to validate this functionality.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_ventilator_validation\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\ventilator_scenarios\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F6F837-0653-43FC-9342-4A846C4DBC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F13C9C1-BF7F-4C91-9325-AEBE28B51016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13245" yWindow="2865" windowWidth="27585" windowHeight="26235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28110" yWindow="5610" windowWidth="25995" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenarios" sheetId="35" r:id="rId1"/>
+    <sheet name="Summary" sheetId="37" r:id="rId1"/>
+    <sheet name="Scenarios" sheetId="35" r:id="rId2"/>
+    <sheet name="Recruitment" sheetId="36" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Scenarios!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Scenarios!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="123">
   <si>
     <t>|</t>
   </si>
@@ -273,6 +275,135 @@
   </si>
   <si>
     <t>Mode: PC-CMV&lt;br&gt;Inspiratory Pressure Target: set empirically to achieve VT Target&lt;br&gt;VT Target (mL/kg): 9.0&lt;br&gt;VT Target (mL): 678&lt;br&gt;PEEP (cm H2O): 8&lt;br&gt;FiO2 (%): 40&lt;br&gt;Mandatory Rate (bpm): 15&lt;br&gt;I:E: 0.43&lt;br&gt;Minute Ventilation (L/min): 10.2&lt;br&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario </t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Decent</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="warning"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="danger"&gt;</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Mild ARDS</t>
+  </si>
+  <si>
+    <t>Moderate ARDS</t>
+  </si>
+  <si>
+    <t>Severe ARDS</t>
+  </si>
+  <si>
+    <t>Mild COPD</t>
+  </si>
+  <si>
+    <t>Moderate COPD</t>
+  </si>
+  <si>
+    <t>Severe COPD</t>
+  </si>
+  <si>
+    <t>Healthy PC-CMV</t>
+  </si>
+  <si>
+    <t>Healthy VC-CMV</t>
+  </si>
+  <si>
+    <t>Healthy VC-AC</t>
+  </si>
+  <si>
+    <t>PC-CMV with Severity = 0.3</t>
+  </si>
+  <si>
+    <t>PC-CMV with Severity = 0.6</t>
+  </si>
+  <si>
+    <t>PC-CMV with Severity = 0.9</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Increase PEEP for improved recruitment</t>
+  </si>
+  <si>
+    <t>PC-CMV mode</t>
+  </si>
+  <si>
+    <t>VC-CMV mode</t>
+  </si>
+  <si>
+    <t>VC-AC mode</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Action Occurrence Time (s)</t>
+  </si>
+  <si>
+    <t>Sampled Scenario Time (s)</t>
+  </si>
+  <si>
+    <t>Ventilate patient with moderate ARDS</t>
+  </si>
+  <si>
+    <t>Apneic and intubated; VC-CMV: RR = 15 bpm, I:E = 0.6, TV = 7 mL/kg(ideal), FIO2 = 0.5, PEEP = 5.0 cmH2O</t>
+  </si>
+  <si>
+    <t>Increase PEEP</t>
+  </si>
+  <si>
+    <t>PEEP = 20.0 cmH2O</t>
+  </si>
+  <si>
+    <t>Pulmonary Shunt (%)</t>
+  </si>
+  <si>
+    <t>33 +/- 15 @cite karbing2020changes</t>
+  </si>
+  <si>
+    <t>22 +/- 14 @cite karbing2020changes</t>
+  </si>
+  <si>
+    <t>Horowitz Index (mmHg)</t>
+  </si>
+  <si>
+    <t>130 +/- 58 @cite karbing2020changes</t>
+  </si>
+  <si>
+    <t>220 +/- 82 @cite karbing2020changes</t>
+  </si>
+  <si>
+    <t>Increase @cite karbing2020changes</t>
+  </si>
+  <si>
+    <t>No Change @cite musch2008relation</t>
+  </si>
+  <si>
+    <t>Arterial Carbon Dioxide Partial Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>Arterial Oxygen Partial Pressure (mmHg)</t>
   </si>
 </sst>
 </file>
@@ -603,7 +734,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -744,6 +875,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -789,7 +933,7 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -800,41 +944,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -900,9 +1047,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -940,9 +1087,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -975,26 +1122,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1027,26 +1157,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1219,38 +1332,523 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648268E1-5318-457A-AD23-EE7F0793B562}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="137.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>8</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10">
+        <f>SUM(F3:F12)</f>
+        <v>107</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="11">
+        <f>SUM(H3:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="12">
+        <f>SUM(J3:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="33.85546875" style="15" customWidth="1"/>
-    <col min="20" max="20" width="30" style="11" customWidth="1"/>
-    <col min="21" max="21" width="33.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="33.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="30" style="1" customWidth="1"/>
+    <col min="21" max="21" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="33" style="10" customWidth="1"/>
-    <col min="24" max="24" width="30.5703125" style="11" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.5703125" style="11" customWidth="1"/>
-    <col min="27" max="27" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1270,16 +1868,16 @@
       <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1288,34 +1886,34 @@
       <c r="K1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -1327,7 +1925,7 @@
       <c r="X1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="Z1" s="4" t="s">
@@ -1337,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1353,67 +1951,67 @@
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="13" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="13" t="s">
+      <c r="S2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" s="8" t="s">
+      <c r="U2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Y2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="AA2" s="7" t="s">
@@ -1436,52 +2034,52 @@
       <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="9" t="s">
+      <c r="O3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T3" s="9" t="s">
+      <c r="S3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="V3" s="6" t="s">
@@ -1490,13 +2088,13 @@
       <c r="W3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="9" t="s">
+      <c r="Y3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="AA3" s="7" t="s">
@@ -1504,680 +2102,668 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="K4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="M4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="9" t="s">
+      <c r="O4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" s="9" t="s">
+      <c r="Q4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T4" s="9" t="s">
+      <c r="S4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V4" s="9" t="s">
+      <c r="U4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X4" s="9" t="s">
+      <c r="W4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Y4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Y4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="9" t="s">
+      <c r="K5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="9" t="s">
+      <c r="O5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="9" t="s">
+      <c r="Q5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="9" t="s">
+      <c r="S5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="U5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X5" s="9" t="s">
+      <c r="W5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Y5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Y5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AA5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="9" t="s">
+      <c r="I6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="9" t="s">
+      <c r="M6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="9" t="s">
+      <c r="O6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="9" t="s">
+      <c r="Q6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T6" s="9" t="s">
+      <c r="S6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V6" s="9" t="s">
+      <c r="U6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X6" s="9" t="s">
+      <c r="W6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Y6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="9" t="s">
+      <c r="Y6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AA6" s="12" t="s">
+      <c r="AA6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="I7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="9" t="s">
+      <c r="M7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="9" t="s">
+      <c r="O7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="9" t="s">
+      <c r="Q7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="9" t="s">
+      <c r="S7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="U7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="9" t="s">
+      <c r="U7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="W7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" s="9" t="s">
+      <c r="W7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Y7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="9" t="s">
+      <c r="Y7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AA7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="9" t="s">
+      <c r="I8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="9" t="s">
+      <c r="K8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="9" t="s">
+      <c r="M8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="9" t="s">
+      <c r="O8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="9" t="s">
+      <c r="Q8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T8" s="9" t="s">
+      <c r="S8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" s="9" t="s">
+      <c r="U8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X8" s="9" t="s">
+      <c r="W8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="Y8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="9" t="s">
+      <c r="Y8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AA8" s="12" t="s">
+      <c r="AA8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="I9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="9" t="s">
+      <c r="K9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="9" t="s">
+      <c r="M9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="9" t="s">
+      <c r="O9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="9" t="s">
+      <c r="Q9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="S9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="9" t="s">
+      <c r="S9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="U9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V9" s="9" t="s">
+      <c r="U9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X9" s="9" t="s">
+      <c r="W9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Y9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="9" t="s">
+      <c r="Y9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AA9" s="12" t="s">
+      <c r="AA9" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="I10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="9" t="s">
+      <c r="K10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="9" t="s">
+      <c r="M10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="9" t="s">
+      <c r="O10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="9" t="s">
+      <c r="Q10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="S10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="9" t="s">
+      <c r="S10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V10" s="9" t="s">
+      <c r="U10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X10" s="9" t="s">
+      <c r="W10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Y10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="9" t="s">
+      <c r="Y10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AA10" s="12" t="s">
+      <c r="AA10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="9" t="s">
+      <c r="I11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="9" t="s">
+      <c r="K11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="O11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="9" t="s">
+      <c r="O11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="9" t="s">
+      <c r="Q11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="S11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="9" t="s">
+      <c r="S11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="U11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="9" t="s">
+      <c r="U11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="W11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="X11" s="9" t="s">
+      <c r="W11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Y11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="9" t="s">
+      <c r="Y11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AA11" s="12" t="s">
+      <c r="AA11" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -2188,4 +2774,251 @@
     <oddHeader>&amp;L&amp;A</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76643D9A-8B3E-4F63-82A7-E6D6266B9D51}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="2" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="2" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="2" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="15" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" style="15" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="15" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" style="15" customWidth="1"/>
+    <col min="17" max="17" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16">
+        <v>330</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>330</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>630</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed ventilator validation table formatting issue.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/MechanicalVentilatorValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\ventilator_scenarios\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F13C9C1-BF7F-4C91-9325-AEBE28B51016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D11331-4AE1-4920-87DC-24509310866A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28110" yWindow="5610" windowWidth="25995" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26820" yWindow="2715" windowWidth="29925" windowHeight="24645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="37" r:id="rId1"/>
@@ -373,9 +373,6 @@
     <t>Increase PEEP</t>
   </si>
   <si>
-    <t>PEEP = 20.0 cmH2O</t>
-  </si>
-  <si>
     <t>Pulmonary Shunt (%)</t>
   </si>
   <si>
@@ -404,6 +401,9 @@
   </si>
   <si>
     <t>Arterial Oxygen Partial Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>PEEP = 15.0 cmH2O</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648268E1-5318-457A-AD23-EE7F0793B562}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1823,8 +1823,8 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,8 +2780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76643D9A-8B3E-4F63-82A7-E6D6266B9D51}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,25 +2835,25 @@
         <v>0</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>0</v>
@@ -2941,25 +2941,25 @@
         <v>1</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>3</v>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>0</v>
@@ -2994,25 +2994,25 @@
         <v>1</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="14" t="s">
+      <c r="O4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>3</v>

</xml_diff>